<commit_message>
modified News_classification_model.py with try-except block
</commit_message>
<xml_diff>
--- a/News_dataset.xlsx
+++ b/News_dataset.xlsx
@@ -26,6 +26,12 @@
     <t>class</t>
   </si>
   <si>
+    <t>Jaipur Rajasthan performed spectacularly NEET National Eligibility cum Entrance Tests exam year Out 79,057 appeared NEET 45,336 candidates cleared test 182 Jaipur alone four top 50 state.Prince Chaudhary small village Barmer The 17-year-old became famous overnight securing fifth rank country Son medical store owner Prince wants pursue medical course All India Institute Medical Science Delhi become neuro physician `` happy shy teenager told NDTV And though studied Hindi medium school till class 10 two years intense coaching career institute Kota gave confidence take exam English scoring 686 720.Not Prince one every five students polished exam skills coaching centres Kota claims one teachers institute `` Coaching institutes create awareness able help students focused preparation said Naveen Maheshwari heads one sought coaching institutes Kota The city famous cotton sarees seen mushrooming coaching centres thriving NEET boom There around 1.5 lakh students 150 centres city.googletag.cmd.push function googletag.display `` adslotNativeVideo Students mostly enroll institutes class 11 spend two years studying exactly crack exam says Manan Bhardwaj Jaipur got India rank 150 `` It matter much study matters study Manan told NDTV Comments We seeing child Barmer cleared exam also got India rank 5 unheard till years ago Last year saw Rupa Yadav child bride married 8 clear exam So certainly awareness coaching help children back ground Mr Maheshwari said.In coaching capital 150 institutes annual turnover Rs 1500 crore say reports And 's tuition fees lakhs aspirants come Uttar Pradesh Madhya Pradesh Chhattisgarh Bihar parts northern India rent rooms duration courses There booming PG accommodation business private houses dormitories facilities</t>
+  </si>
+  <si>
+    <t>news</t>
+  </si>
+  <si>
     <t>Netflix made name back really good TV shows continues spend billions dollars year build portfolio original series prominently showcases homepage attract eyeballs self-produced efforts By tends background popular critically-acclaimed series n't make arguably better anything Netflix made history.There 's need highlight casual viewers may miss Netflix 's 've taken upon gather best TV shows streaming Netflix To prepare list used aggregate ratings Rotten Tomatoes Metacritic IMDb draw shortlist picked top 50 Here best TV shows Netflix India sorted alphabetically This list updated every month worthy additions movies removed service bookmark page keep checking in.The 100 Best Movies Netflix India A Series Unfortunate Events 2017 – Present Three resourceful orphans – inventor reader baby sharp teeth – must outsmart evil distant relative 's sizeable fortune trying uncover mystery behind secret society parents involved Based Lemony Snicket 's popular series children 's books Alias Grace 2017 Margaret Atwood 's 1996 novel name 19th-century Canadian woman convicted double murder becomes subject criminal psychologist – profession n't exist name – adapted screen six-part miniseries American Crime Story 2016 – Present A true crime anthology series prolific producer Ryan Murphy follows well-known events dominated US media trial former sportsman O.J Simpson assassination fashion designer Gianni Versace Better Call Saul 2015 – Present This spin-off prequel Breaking Bad follows small-time lawyer Bob Odenkirk tendencies con artist transforms morally-challenged criminal lawyer knew Saul Goodman Black Mirror 2011 – Present Charlie Brooker 's anthology series consisting standalone episodes – means ever-changing cast addition new settings storylines – explores unanticipated consequences new technologies often dark satirical ways BoJack Horseman 2014 – Present Set world humans anthropomorphic animals live alongside washed-up sitcom star plans comeback fame help ghostwriter ex-girlfriend 's also agent freeloading roommate dealing rival 's dating ghostwriter Breaking Bad 2008 – 2013 Diagnosed lung cancer struggling high school chemistry teacher Bryan Cranston decides get business making selling meth secure family 's financial future help former student Aaron Paul Broadchurch 2013 – 2017 A look violent crimes affect small seaside town Britain eyes two investigators David Tennant Olivia Colman impact media attention suspicion grief close-knit community Brooklyn Nine-Nine 2013 – Present The lives group detectives fictional New York precinct – ensemble featuring Any Samberg AndreBraugher Terry Crews – get sitcom treatment The Office co-creator Michael Schur Crazy Ex-Girlfriend 2015 – Present A successful young female lawyer Rachel Bloom also co-creator suffers depression anxiety uproots life New York moves suburb California find love happiness The Crown 2016 – Present A look life Britain 's longest-ruling monarch Queen Elizabeth II wedding 1947 present day including political rivalries romances world-changing events reign Daredevil 2015 – Present A blind man fights injustice attorney day masked vigilante night present-day New York struggling deal Catholic guilt arises actions Dear White People 2017 – Present Set fictional predominantly white Ivy League college Justin Simien turns successful satirical film broader series black students dealing social injustice figuring The End F***ing World 2017 – Present Two teenage outsiders – budding psychopath rebel hungry adventure – embark road trip search latter 's real father become involved series increasingly violent events The Expanse 2015 – Present Hundreds years future mankind colonised Solar System brink war 's crew different origins – Earth Mars Asteroid Belt – expose greatest conspiracy Fargo 2014 – Present The Coen brothers acclaimed film name inspiration black comedy/crime anthology series featuring quirky characters across different eras dealing deception intrigue murder amidst cold American Midwest Fauda 2015 – Present A former expert Israeli agent comes retirement hunt Palestinian militant show cleverly following sides conflict drawing real world events Fullmetal Alchemist Brotherhood 2009 – 2010 This direct adaptation famous manga centres two brothers looking Philosopher 's Stone restore bodies failed experimental attempt resurrect mother goes awry But 're ones stone GLOW 2017 – Present An exploration real-life 1980s women 's professional wrestling – Gorgeous Ladies Of Wresting GLOW – focusing personal professional lives fictionalised Hollywood misfits involved Godless 2017 In 19th century murderous outlaw notorious gang hunt ex-protégé betrayed find conflict town gives refuge whose residents mainly women A seven-episode miniseries The Good Place 2016 – Present The Office co-creator Michael Schur spun sitcom web afterlife series following woman Kristen Bell 's mistakenly assigned Heaven-like utopia tries better person hide The Good Wife 2009 – 2016 After humiliating sex corruption scandal puts husband behind bars wife – former state 's attorney – must return work provide family battling unwanted spotlight Hannibal 2013 – 2015 Cancelled three seasons cult horror hit explores relationship forensic psychiatrist Mads Mikkelsen patient young FBI criminal profiler uncanny ability empathise serial killers Happy Valley 2014 – Present A British police sergeant dealing personal problems investigates cases small West Yorkshire town Two seasons six episodes possibly way House Cards 2013 – Present A betrayed US Congressman works equally conniving wife climb political ladders Washington anything needed – manipulation deceit even murder – achieve goals The Inbetweeners 2008 – 2010 A coming-of-age sitcom whose success led two movies following four British teenagers final year school series misadventures involving uncaring school staff male bonding failed sexual encounters Jane Virgin 2014 – Present Gina Rodriguez Annihilation stars devout Catholic working young Latina virgin becomes pregnant accidental artificial insemination rom-com satire end fifth season 2019 Jessica Jones 2015 – Present Suffering PTSD super-powered woman rebuilds life private investigator New York forced battle past demons every step way wants look past Lost 2004 – 2010 The survivors plane crash must work together survive mysterious tropical island somewhere South Pacific Ocean battling supernatural sci-fi elements Faltered midway recovered ended disappointing fashion Luther 2010 – Present Idris Elba stars dedicated brilliant British detective tries keep grip personal life dealing psychological fallouts crimes 's tasked solve Mad Men 2007 – 2015 Set 1960s New York slow-burn drama offers peek inside fictional ad agency focusing one extremely talented executives Jon Hamm 's bored simple personal life Master None 2015 – Present Loosely based Aziz Ansari 's life experiences 30-year-old struggling actor tries get life order personal professional fronts affected Indian ancestry Mindhunter 2017 – Present In late 1970s two FBI agents push superiors expand research criminal science involves getting close personal imprisoned serial killers understand think Monty Python 's Flying Circus 1969 – 1974 The influential British comedy group got start surreal sketch series targeted life island intellectual fashion humour wide-ranging unique gave birth term `` Pythonesque Narcos 2015 – Present A gripping look violent powerful drug cartels Colombia including infamous Pablo Escobar thecorroborative efforts various law enforcement whose job bring Orange Is New Black 2013 – Present The lives incarcerated women minimum-security federal prison upstate New York including normally law-abiding privileged woman 's sentenced decade-old crime Orphan Black 2013 – 2017 A con artist Tatiana Maslany assumes identity woman committed suicide looked like pulled conspiracy learns 's clone Outlander 2014 – Present Diana Gabaldon 's best-selling books married nurse World War II 's transported back time 1743 finds caught Jacobite risings two different men Peaky Blinders 2013 – Present The exploits Shelby crime family Birmingham England two World Wars elements borrowed 19th-century gang name legend goes used sew razor blades caps Peep Show 2003 – 2015 The lives two different dysfunctional twenty-somethings sharing flat South London day-to-day farcical antics made cult favourite Rick Morty 2013 – Present An adult animated sci-fi series cynical alcoholic mad scientist Rick weak-willed easily influenced grandson Morty go series misadventures across dimensions universes Sherlock 2010 – Present Benedict Cumberbatch Martin Freeman play famous detective doctor sidekick modern-day adaptation Sir Arthur Conan Doyle 's stories Terrific compelling first years though derailed fourth season Star Trek 1966 – 1969 Gene Rodenberry 's original series adventures starship 2260s led Kirk Spock McCoy n't age well visually storytelling endures set aside major dip quality third season Star Trek The Next Generation 1987 – 1994 Rodenberry took vision even far-off future – 24th century – focusing new generation Starfleet officers new ship recognisable name Stranger Things 2016 – Present A nostalgia-heavy love letter 80s set suburban small town secret scientific experiments paranormal supernatural times human subjects starts wreak havoc normal lives residents That '70s Show 1997 – 2006 The comedy fueled Hollywood careers stars Mila Kunis Ashton Kutcher group six high school friends going usual teenage problems trying figure identities Trollhunters 2016 – Present Guillermo del Toro turns love monster stories animated series ages following teenage boy stumbles onto mystic amulet must protect world humans trolls Unbreakable Kimmy Schmidt 2015 – Present Rescued doomsday cult 15 years young woman armed positive attitude decides start new life New York help gay wannabe-Broadway actor roommate street-wise landlady depressed out-of-touch socialite The Walking Dead 2010 – Present Based popular comic series horror drama set post-apocalyptic future survivors search safe world overrun zombies Hit peak fifth season never recovered Wentworth 2013 – Present Locked awaiting trial attempted murder husband woman adjusts life Australian prison rises ranks Gripping till season 4 post lead actress left div class='compare-product-widget /div</t>
   </si>
   <si>
@@ -35,9 +41,6 @@
     <t>New Delhi TIMES Higher Education THE World University Ranking released rankings educational institutes Asia two Indian institutes made way top 50 Asian institutes The two institutes made way top 50 Indian Institute Science 29th place Indian Institute Technology Bombay 44th rank Other institutes made way top 100 Indian Institute Technology Kharagpur Indian Institute Technology Roorkee Indian Institute Technology Kanpur Indian Institute Technology Delhi The ranks released THE World University Ranking Indian Institute Science IISc world rank 29Indian Institute Technology IIT Bombay world rank 44Indian Institute Technology IIT Kharagpur world rank 60Indian Institute Technology IIT Roorkee world rank 65Indian Institute Technology IIT Kanpur world rank 81Indian Institute Technology IIT Delhi world rank 86Among made top 200 Tezpur University 100th place Indian Institute Technology Madras 103rd place Indian Institute Technology Guwahati 112th place Panjab University 114th place National Institute Technology Rourkela 126th place Jadavpur University 127th place Indian School Mines 141st place University Delhi 144th place Aligarh Muslim University 158th place Savitribai Phule Pune University 188th place IIT-BHU 194th place CommentsA total 17 institutes India made way top 200 Asian Universities Though representation India increased list several universities fallen rankings comparison last year Both IISc IIT Bombay dropped two places 29th 44th position respectively IIT Madras witnessed biggest decline year fallen last year 's 41st place 103rd pace year googletag.cmd.push function googletag.display `` adslotNativeVideo Click Education News</t>
   </si>
   <si>
-    <t>news</t>
-  </si>
-  <si>
     <t>New Delhi A differently abled Indian teacher little-known institution Uttarakhand beat tough competition around world named today among top 50 contenders USD 1 million global award Pradeep Negi economics social science computer science teacher Government Inter College BHEL Ranipur Haridwar shortlisted annual Varkey Foundation Global Teacher Prize 2018 30,000 nominations applications 173 countries around world `` It unbelievable proud chosen one top 50 teachers It motivated teachers community said Mr Negi `` handicapped n't stopped succeeding glad inspire disabled people India developed lot innovative work ICT poor children glad recognised said Mr Negi physically disabled age two due polio.Read Maggie McDonnell Teacher From Canada Wins Global Teacher Prize 2017Negi chosen fighting spirit suffered bullying school disability overcoming adversities use new technology tools make economics social subjects compelling students.googletag.cmd.push function googletag.display `` adslotNativeVideo Congratulations Pradeep Negi reaching final 50 hope story inspires looking enter teaching profession shines spotlight incredible work teachers world every day said Sunny Varkey founder Varkey Foundation Global Teacher Prize `` We intend keep momentum going journey continues return teachers rightful position one respected professions society said.Mr Negi helped train 1,200 teachers state.The Global Teacher Prize set recognise one exceptional teacher every year made outstanding contribution profession.The top 50 shortlisted teachers narrowed 10 finalists committee results announced February 2018.The winner chosen final 10 finalists Global Teacher Prize Academy.All 10 finalists invited Dubai Award ceremony Global Education Skills Forum GESF March 18 2018 winner announced live stage CommentsClick Education News Except headline story edited NDTV staff published syndicated feed</t>
   </si>
   <si>
@@ -75,9 +78,6 @@
   </si>
   <si>
     <t>New Delhi Enthused success SBI merger Finance Ministry considering clearing another proposal public sector banking space fiscal end goal create 4-5 global sized lenders.Five associate banks Bharatiya Mahila Bank became part SBI April 1 2017 catapulting country 's largest lender among top 50 banks world.Now Finance Ministry looking replicate model case state-run banks reach critical mass compete global peers `` Consolidation must ... decision regard would based commercially prudent parameters If NPA situation gets better could one merger towards end fiscal senior official told PTI.Toxic loans public sector banks rose Rs 1 lakh crore Rs 6.06 lakh crore April-December 2016-17 bulk came power steel road infrastructure textile sectors.Finance Minister Arun Jaitley several occasions said India needs 5-6 banks global size scale consolidation banking sector done appropriate time.googletag.cmd.push function googletag.display `` adslotNativeVideo Whenever consolidation happens takes consideration interest stakeholders including employees shareholders official said adding win-win parties.A balancing act done merger given clearance various authorities regulators official added.The future merger proposals banking sector also require clearance Competition Commission India CCI see merged entity going create monopoly.In last consolidation drive saw light day April CCI nod needed case merger Bharatiya Mahila Bank BMB SBI There requirement merger associate banks SBI part parent.The Finance Ministry sought help government think-tank NITI Aayog global consultancy firms examine possibility next round consolidation PSU banks aim create lenders global size scale.NITI Aayog 's report expected set tone roadmap consolidation future.There factors like regional balance geographical reach financial burden smooth human resource transition looked taking merger decision official said.The official added merger weak bank strong bank `` could pull latter `` There low-hanging fruits Big lenders like Bank Baroda take turnaround banks southern region Indian Overseas Bank Dena Bank could merged large South Indian bank official explained.Five associates BMB became part SBI April 1 2017 catapulting country 's largest lender among top 50 banks world.State Bank Bikaner Jaipur SBBJ State Bank Hyderabad SBH State Bank Mysore SBM State Bank Patiala SBP State Bank Travancore SBT besides BMB merged SBI.With merger total customer base SBI reached around 37 crore branch network around 24,000 nearly 59,000 ATMs across country The merged entity began operation deposit base Rs 26 lakh crore advances Rs 18.50 lakh crore CommentsThe government February approved merger five associate banks SBI Later March cabinet approved merger BMB well SBI first merged State Bank Saurashtra 2008 Two years later State Bank Indore merged This story edited NDTV staff auto-generated syndicated feed</t>
-  </si>
-  <si>
-    <t>HighlightsThree Indian companies list world 's top 50 luxury goods firms Gitanjali Gems ranked 30th Global Powers Luxury Goods list Other two Indian companies list Titan Company PC Jewellerwindow._pricee window._pricee || _pricee.push container '_pcwgtmid New Delhi Gitanjali Gems Titan PC Jeweller three Indian companies named list top 50 luxury goods firms globally While list topped France-based Louis Vuitton Gitanjali Gems ranked 30th followed Titan Company 31st PC Jeweller 44th Among top 10 companies globally fourth annual Global Powers Luxury Goods report titled 'The new luxury consumer three luxury conglomerates participating multiple sectors luxury good market The fourth annual Global Powers Luxury Goods report examines lists 100 largest luxury goods companies globally based publicly available data consolidated sales luxury goods 2014 -2015 The top three companies LVMH Moet Hennessy-Louis Vuitton SA Louis Vuitton Bulgari Emilio Pucci DonnaKaran TAGHeuer Compaigne Financiere Richemont SA Cartier Van Cleef Arpels Montblanc Chloe The Estee Lauder Companies Inc Estee Lauder M.A.C. Aramis Clinique Aveda Jo Malone .On economic outlook luxury market India potential impact may brands Deloitte India spokesperson said `` A rapidly rising urban middle class increasing disposable income expected drive sales luxury goods The demand luxury goods expected remain strong India remains bright spot among Asian BRIC countries despite tax luxury goods `` googletag.cmd.push function googletag.display `` adslotNativeVideo CommentsEmerging consumer markets continue drive luxury market growth In China Russia United Arab Emirates categorised emerging luxury markets 70 per cent consumers claimed increased spending last five years compared 53 per cent mature markets EU US Japan .The report noted world 's 100 largest luxury goods companies generated sales 212 billion 2014-15 The average luxury goods annual sales top 100 company stood 2.1 billion</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -473,7 +473,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -495,7 +495,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -517,7 +517,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -525,10 +525,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
         <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -539,7 +539,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -550,7 +550,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -561,7 +561,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -572,7 +572,7 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -583,7 +583,7 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -594,7 +594,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -627,7 +627,7 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -638,7 +638,7 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -660,7 +660,7 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -682,7 +682,7 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -690,10 +690,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
         <v>14</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -704,7 +704,7 @@
         <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -715,7 +715,7 @@
         <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -726,7 +726,7 @@
         <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -737,7 +737,7 @@
         <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -748,7 +748,7 @@
         <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -759,7 +759,7 @@
         <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>